<commit_message>
Foi resolvido onde coloca os dados de consumo e Valor Fatura  na planilha
</commit_message>
<xml_diff>
--- a/BALANÇO_COMPLETO.xlsx
+++ b/BALANÇO_COMPLETO.xlsx
@@ -9,7 +9,6 @@
     <sheet name="RESUMO " sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="UC GERADORA" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="UC BENEF. 1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="UC GERADORA 2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -1752,12 +1751,12 @@
       </c>
       <c r="F7" s="11" t="inlineStr">
         <is>
-          <t>16361337</t>
+          <t>200027499</t>
         </is>
       </c>
       <c r="G7" s="12" t="inlineStr">
         <is>
-          <t>AVENIDA ALPHAVILLE FLAMBOYANT, N. 208 RESIDENCIAL HOUSING FLAMBOYANT</t>
+          <t>RUA CARAI, Q. 12, L. 15, S/N PARQUE ITATIAIA</t>
         </is>
       </c>
       <c r="H7" s="158" t="n"/>
@@ -1786,12 +1785,12 @@
       </c>
       <c r="F8" s="8" t="inlineStr">
         <is>
-          <t>2025003047807</t>
+          <t>10031998761</t>
         </is>
       </c>
       <c r="G8" s="165" t="inlineStr">
         <is>
-          <t>AVENIDA CASTELO BRANCO, Q. 38, L. 40, S/N SETOR COIMBRA</t>
+          <t>RUA K-4, Q. 01, L. 10, S/N JARDIM ESPLANADA</t>
         </is>
       </c>
       <c r="H8" s="158" t="n"/>
@@ -1824,16 +1823,8 @@
       <c r="E9" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>11844589</t>
-        </is>
-      </c>
-      <c r="G9" s="165" t="inlineStr">
-        <is>
-          <t>AVENIDA FUED JOSE SEBBA, Q. A 23, L. 12, N. 626, APART - 201, COND - RESID SERRA DOURADA, - - 4 JARDIM GOIAS</t>
-        </is>
-      </c>
+      <c r="F9" s="8" t="n"/>
+      <c r="G9" s="165" t="n"/>
       <c r="H9" s="158" t="n"/>
       <c r="I9" s="66" t="n"/>
       <c r="J9" s="4">
@@ -2493,12 +2484,12 @@
       </c>
       <c r="B5" s="74" t="inlineStr">
         <is>
-          <t>27/12/2024</t>
+          <t>19/12/2024</t>
         </is>
       </c>
       <c r="C5" s="74" t="inlineStr">
         <is>
-          <t>27/01/2025</t>
+          <t>18/01/2025</t>
         </is>
       </c>
       <c r="D5" s="35">
@@ -2515,13 +2506,13 @@
         <v/>
       </c>
       <c r="I5" s="28" t="n">
-        <v>829</v>
+        <v>226</v>
       </c>
       <c r="J5" s="28" t="n">
-        <v>845</v>
+        <v>181</v>
       </c>
       <c r="K5" s="28" t="n">
-        <v>945</v>
+        <v>211</v>
       </c>
       <c r="L5" s="73">
         <f>(K5+(E5-I5))</f>
@@ -2532,25 +2523,25 @@
         <v/>
       </c>
       <c r="N5" s="180" t="n">
-        <v>103.93</v>
+        <v>27.39</v>
       </c>
       <c r="O5" s="35">
         <f>I5-J5</f>
         <v/>
       </c>
       <c r="P5" s="28" t="n">
-        <v>277</v>
+        <v>1418</v>
       </c>
       <c r="R5" s="146" t="inlineStr">
         <is>
-          <t>13168154-1</t>
+          <t>12378019-5</t>
         </is>
       </c>
       <c r="S5" s="146" t="n">
-        <v>20836</v>
+        <v>16289</v>
       </c>
       <c r="T5" s="146" t="n">
-        <v>21781</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="6">
@@ -2561,12 +2552,12 @@
       </c>
       <c r="B6" s="55" t="inlineStr">
         <is>
-          <t>27/01/2025</t>
+          <t>18/01/2025</t>
         </is>
       </c>
       <c r="C6" s="74" t="inlineStr">
         <is>
-          <t>25/02/2025</t>
+          <t>17/02/2025</t>
         </is>
       </c>
       <c r="D6" s="35">
@@ -2580,13 +2571,13 @@
       </c>
       <c r="H6" s="181" t="n"/>
       <c r="I6" s="28" t="n">
-        <v>825</v>
+        <v>273</v>
       </c>
       <c r="J6" s="28" t="n">
-        <v>685</v>
+        <v>160</v>
       </c>
       <c r="K6" s="28" t="n">
-        <v>785</v>
+        <v>190</v>
       </c>
       <c r="L6" s="73">
         <f>(K6+(E6-I6))</f>
@@ -2597,25 +2588,25 @@
         <v/>
       </c>
       <c r="N6" s="180" t="n">
-        <v>0</v>
+        <v>34.19</v>
       </c>
       <c r="O6" s="35">
         <f>I6-J6</f>
         <v/>
       </c>
       <c r="P6" s="28" t="n">
-        <v>542.5</v>
+        <v>1531</v>
       </c>
       <c r="R6" s="140" t="inlineStr">
         <is>
-          <t>13168154-1</t>
+          <t>12378019-5</t>
         </is>
       </c>
       <c r="S6" s="140" t="n">
-        <v>21781</v>
+        <v>16500</v>
       </c>
       <c r="T6" s="140" t="n">
-        <v>22566</v>
+        <v>16690</v>
       </c>
     </row>
     <row r="7">
@@ -2624,11 +2615,16 @@
           <t>Mar</t>
         </is>
       </c>
-      <c r="B7" s="55">
-        <f>C6</f>
-        <v/>
-      </c>
-      <c r="C7" s="74" t="n"/>
+      <c r="B7" s="55" t="inlineStr">
+        <is>
+          <t>17/02/2025</t>
+        </is>
+      </c>
+      <c r="C7" s="74" t="inlineStr">
+        <is>
+          <t>19/03/2025</t>
+        </is>
+      </c>
       <c r="D7" s="35">
         <f>'RESUMO '!B16</f>
         <v/>
@@ -2639,9 +2635,15 @@
         <v/>
       </c>
       <c r="H7" s="181" t="n"/>
-      <c r="I7" s="28" t="n"/>
-      <c r="J7" s="28" t="n"/>
-      <c r="K7" s="28" t="n"/>
+      <c r="I7" s="28" t="n">
+        <v>204</v>
+      </c>
+      <c r="J7" s="28" t="n">
+        <v>282</v>
+      </c>
+      <c r="K7" s="28" t="n">
+        <v>312</v>
+      </c>
       <c r="L7" s="73">
         <f>(K7+(E7-I7))</f>
         <v/>
@@ -2650,15 +2652,27 @@
         <f>IFERROR(L7/$H$5,"")</f>
         <v/>
       </c>
-      <c r="N7" s="180" t="n"/>
+      <c r="N7" s="180" t="n">
+        <v>52.61</v>
+      </c>
       <c r="O7" s="35">
         <f>I7-J7</f>
         <v/>
       </c>
-      <c r="P7" s="28" t="n"/>
-      <c r="R7" s="140" t="n"/>
-      <c r="S7" s="140" t="n"/>
-      <c r="T7" s="140" t="n"/>
+      <c r="P7" s="28" t="n">
+        <v>1453</v>
+      </c>
+      <c r="R7" s="140" t="inlineStr">
+        <is>
+          <t>12378019-5</t>
+        </is>
+      </c>
+      <c r="S7" s="140" t="n">
+        <v>16690</v>
+      </c>
+      <c r="T7" s="140" t="n">
+        <v>17002</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="122" t="inlineStr">
@@ -2668,12 +2682,12 @@
       </c>
       <c r="B8" s="55" t="inlineStr">
         <is>
-          <t>27/03/2025</t>
+          <t>19/03/2025</t>
         </is>
       </c>
       <c r="C8" s="74" t="inlineStr">
         <is>
-          <t>26/04/2025</t>
+          <t>16/04/2025</t>
         </is>
       </c>
       <c r="D8" s="35">
@@ -2687,13 +2701,13 @@
       </c>
       <c r="H8" s="181" t="n"/>
       <c r="I8" s="28" t="n">
-        <v>697</v>
+        <v>155</v>
       </c>
       <c r="J8" s="28" t="n">
-        <v>887</v>
+        <v>179</v>
       </c>
       <c r="K8" s="28" t="n">
-        <v>987</v>
+        <v>209</v>
       </c>
       <c r="L8" s="73">
         <f>(K8+(E8-I8))</f>
@@ -2704,25 +2718,25 @@
         <v/>
       </c>
       <c r="N8" s="180" t="n">
-        <v>113.45</v>
+        <v>44.52</v>
       </c>
       <c r="O8" s="35">
         <f>I8-J8</f>
         <v/>
       </c>
       <c r="P8" s="28" t="n">
-        <v>594</v>
+        <v>1429</v>
       </c>
       <c r="R8" s="140" t="inlineStr">
         <is>
-          <t>13168154-1</t>
+          <t>12378019-5</t>
         </is>
       </c>
       <c r="S8" s="140" t="n">
-        <v>23377</v>
+        <v>17002</v>
       </c>
       <c r="T8" s="140" t="n">
-        <v>24364</v>
+        <v>17211</v>
       </c>
     </row>
     <row r="9">
@@ -2733,12 +2747,12 @@
       </c>
       <c r="B9" s="55" t="inlineStr">
         <is>
-          <t>26/04/2025</t>
+          <t>16/04/2025</t>
         </is>
       </c>
       <c r="C9" s="74" t="inlineStr">
         <is>
-          <t>28/05/2025</t>
+          <t>15/05/2025</t>
         </is>
       </c>
       <c r="D9" s="35">
@@ -2752,13 +2766,13 @@
       </c>
       <c r="H9" s="181" t="n"/>
       <c r="I9" s="28" t="n">
-        <v>766</v>
+        <v>159</v>
       </c>
       <c r="J9" s="28" t="n">
-        <v>885</v>
+        <v>164</v>
       </c>
       <c r="K9" s="28" t="n">
-        <v>985</v>
+        <v>194</v>
       </c>
       <c r="L9" s="73">
         <f>(K9+(E9-I9))</f>
@@ -2769,25 +2783,25 @@
         <v/>
       </c>
       <c r="N9" s="180" t="n">
-        <v>114.46</v>
+        <v>44.77</v>
       </c>
       <c r="O9" s="35">
         <f>I9-J9</f>
         <v/>
       </c>
       <c r="P9" s="28" t="n">
-        <v>522.5</v>
+        <v>1424</v>
       </c>
       <c r="R9" s="140" t="inlineStr">
         <is>
-          <t>13168154-1</t>
+          <t>12378019-5</t>
         </is>
       </c>
       <c r="S9" s="140" t="n">
-        <v>24364</v>
+        <v>17211</v>
       </c>
       <c r="T9" s="140" t="n">
-        <v>25349</v>
+        <v>17405</v>
       </c>
     </row>
     <row r="10">
@@ -2798,12 +2812,12 @@
       </c>
       <c r="B10" s="55" t="inlineStr">
         <is>
-          <t>28/05/2025</t>
+          <t>15/05/2025</t>
         </is>
       </c>
       <c r="C10" s="74" t="inlineStr">
         <is>
-          <t>26/06/2025</t>
+          <t>16/06/2025</t>
         </is>
       </c>
       <c r="D10" s="35">
@@ -2817,13 +2831,13 @@
       </c>
       <c r="H10" s="181" t="n"/>
       <c r="I10" s="28" t="n">
-        <v>678</v>
+        <v>154</v>
       </c>
       <c r="J10" s="28" t="n">
-        <v>519</v>
+        <v>181</v>
       </c>
       <c r="K10" s="28" t="n">
-        <v>619</v>
+        <v>211</v>
       </c>
       <c r="L10" s="73">
         <f>(K10+(E10-I10))</f>
@@ -2834,25 +2848,25 @@
         <v/>
       </c>
       <c r="N10" s="180" t="n">
-        <v>117.28</v>
+        <v>48.03</v>
       </c>
       <c r="O10" s="35">
         <f>I10-J10</f>
         <v/>
       </c>
       <c r="P10" s="28" t="n">
-        <v>627.5</v>
+        <v>1397</v>
       </c>
       <c r="R10" s="140" t="inlineStr">
         <is>
-          <t>13168154-1</t>
+          <t>12378019-5</t>
         </is>
       </c>
       <c r="S10" s="140" t="n">
-        <v>25349</v>
+        <v>17405</v>
       </c>
       <c r="T10" s="140" t="n">
-        <v>25968</v>
+        <v>17616</v>
       </c>
     </row>
     <row r="11">
@@ -2863,12 +2877,12 @@
       </c>
       <c r="B11" s="55" t="inlineStr">
         <is>
-          <t>26/06/2025</t>
+          <t>16/06/2025</t>
         </is>
       </c>
       <c r="C11" s="74" t="inlineStr">
         <is>
-          <t>25/07/2025</t>
+          <t>18/07/2025</t>
         </is>
       </c>
       <c r="D11" s="35">
@@ -2882,13 +2896,13 @@
       </c>
       <c r="H11" s="181" t="n"/>
       <c r="I11" s="28" t="n">
-        <v>694</v>
+        <v>252</v>
       </c>
       <c r="J11" s="28" t="n">
-        <v>420</v>
+        <v>119</v>
       </c>
       <c r="K11" s="28" t="n">
-        <v>520</v>
+        <v>149</v>
       </c>
       <c r="L11" s="73">
         <f>(K11+(E11-I11))</f>
@@ -2899,25 +2913,25 @@
         <v/>
       </c>
       <c r="N11" s="180" t="n">
-        <v>117.27</v>
+        <v>42.91</v>
       </c>
       <c r="O11" s="35">
         <f>I11-J11</f>
         <v/>
       </c>
       <c r="P11" s="28" t="n">
-        <v>656</v>
+        <v>1530</v>
       </c>
       <c r="R11" s="140" t="inlineStr">
         <is>
-          <t>13168154-1</t>
+          <t>12378019-5</t>
         </is>
       </c>
       <c r="S11" s="140" t="n">
-        <v>25968</v>
+        <v>17616</v>
       </c>
       <c r="T11" s="140" t="n">
-        <v>26488</v>
+        <v>17765</v>
       </c>
     </row>
     <row r="12">
@@ -2928,12 +2942,12 @@
       </c>
       <c r="B12" s="55" t="inlineStr">
         <is>
-          <t>25/07/2025</t>
+          <t>18/07/2025</t>
         </is>
       </c>
       <c r="C12" s="74" t="inlineStr">
         <is>
-          <t>26/08/2025</t>
+          <t>18/08/2025</t>
         </is>
       </c>
       <c r="D12" s="35">
@@ -2947,13 +2961,13 @@
       </c>
       <c r="H12" s="181" t="n"/>
       <c r="I12" s="28" t="n">
-        <v>789</v>
+        <v>147</v>
       </c>
       <c r="J12" s="28" t="n">
-        <v>535</v>
+        <v>368</v>
       </c>
       <c r="K12" s="28" t="n">
-        <v>635</v>
+        <v>398</v>
       </c>
       <c r="L12" s="73">
         <f>(K12+(E12-I12))</f>
@@ -2964,25 +2978,25 @@
         <v/>
       </c>
       <c r="N12" s="180" t="n">
-        <v>118.33</v>
+        <v>46.33</v>
       </c>
       <c r="O12" s="35">
         <f>I12-J12</f>
         <v/>
       </c>
       <c r="P12" s="28" t="n">
-        <v>656</v>
+        <v>1309</v>
       </c>
       <c r="R12" s="140" t="inlineStr">
         <is>
-          <t>13168154-1</t>
+          <t>12378019-5</t>
         </is>
       </c>
       <c r="S12" s="140" t="n">
-        <v>26488</v>
+        <v>17765</v>
       </c>
       <c r="T12" s="140" t="n">
-        <v>27123</v>
+        <v>18163</v>
       </c>
     </row>
     <row r="13">
@@ -2993,12 +3007,12 @@
       </c>
       <c r="B13" s="55" t="inlineStr">
         <is>
-          <t>26/08/2025</t>
+          <t>18/08/2025</t>
         </is>
       </c>
       <c r="C13" s="74" t="inlineStr">
         <is>
-          <t>25/09/2025</t>
+          <t>16/09/2025</t>
         </is>
       </c>
       <c r="D13" s="35">
@@ -3012,13 +3026,13 @@
       </c>
       <c r="H13" s="181" t="n"/>
       <c r="I13" s="28" t="n">
-        <v>1163</v>
+        <v>83</v>
       </c>
       <c r="J13" s="28" t="n">
-        <v>701</v>
+        <v>511</v>
       </c>
       <c r="K13" s="28" t="n">
-        <v>801</v>
+        <v>541</v>
       </c>
       <c r="L13" s="73">
         <f>(K13+(E13-I13))</f>
@@ -3029,25 +3043,25 @@
         <v/>
       </c>
       <c r="N13" s="180" t="n">
-        <v>120.32</v>
+        <v>76.59</v>
       </c>
       <c r="O13" s="35">
         <f>I13-J13</f>
         <v/>
       </c>
       <c r="P13" s="28" t="n">
-        <v>656</v>
+        <v>881</v>
       </c>
       <c r="R13" s="140" t="inlineStr">
         <is>
-          <t>13168154-1</t>
+          <t>12378019-5</t>
         </is>
       </c>
       <c r="S13" s="140" t="n">
-        <v>27123</v>
+        <v>18163</v>
       </c>
       <c r="T13" s="140" t="n">
-        <v>27924</v>
+        <v>18704</v>
       </c>
     </row>
     <row r="14">
@@ -3058,12 +3072,12 @@
       </c>
       <c r="B14" s="55" t="inlineStr">
         <is>
-          <t>25/09/2025</t>
+          <t>16/09/2025</t>
         </is>
       </c>
       <c r="C14" s="74" t="inlineStr">
         <is>
-          <t>27/10/2025</t>
+          <t>16/10/2025</t>
         </is>
       </c>
       <c r="D14" s="35">
@@ -3077,13 +3091,13 @@
       </c>
       <c r="H14" s="181" t="n"/>
       <c r="I14" s="28" t="n">
-        <v>597</v>
+        <v>88</v>
       </c>
       <c r="J14" s="28" t="n">
-        <v>911</v>
+        <v>618</v>
       </c>
       <c r="K14" s="28" t="n">
-        <v>1011</v>
+        <v>648</v>
       </c>
       <c r="L14" s="73">
         <f>(K14+(E14-I14))</f>
@@ -3094,25 +3108,25 @@
         <v/>
       </c>
       <c r="N14" s="180" t="n">
-        <v>127.31</v>
+        <v>85.04000000000001</v>
       </c>
       <c r="O14" s="35">
         <f>I14-J14</f>
         <v/>
       </c>
       <c r="P14" s="28" t="n">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="R14" s="140" t="inlineStr">
         <is>
-          <t>13168154-1</t>
+          <t>12378019-5</t>
         </is>
       </c>
       <c r="S14" s="140" t="n">
-        <v>27924</v>
+        <v>18704</v>
       </c>
       <c r="T14" s="140" t="n">
-        <v>28935</v>
+        <v>19352</v>
       </c>
     </row>
     <row r="15">
@@ -3123,12 +3137,12 @@
       </c>
       <c r="B15" s="55" t="inlineStr">
         <is>
-          <t>27/10/2025</t>
+          <t>16/10/2025</t>
         </is>
       </c>
       <c r="C15" s="74" t="inlineStr">
         <is>
-          <t>26/11/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="D15" s="35">
@@ -3142,13 +3156,13 @@
       </c>
       <c r="H15" s="181" t="n"/>
       <c r="I15" s="28" t="n">
-        <v>919</v>
+        <v>112</v>
       </c>
       <c r="J15" s="28" t="n">
-        <v>651</v>
+        <v>463</v>
       </c>
       <c r="K15" s="28" t="n">
-        <v>751</v>
+        <v>618</v>
       </c>
       <c r="L15" s="73">
         <f>(K15+(E15-I15))</f>
@@ -3159,25 +3173,25 @@
         <v/>
       </c>
       <c r="N15" s="180" t="n">
-        <v>145.54</v>
+        <v>248.92</v>
       </c>
       <c r="O15" s="35">
         <f>I15-J15</f>
         <v/>
       </c>
       <c r="P15" s="28" t="n">
-        <v>342</v>
+        <v>0</v>
       </c>
       <c r="R15" s="140" t="inlineStr">
         <is>
-          <t>13168154-1</t>
+          <t>12378019-5</t>
         </is>
       </c>
       <c r="S15" s="140" t="n">
-        <v>28935</v>
+        <v>19352</v>
       </c>
       <c r="T15" s="140" t="n">
-        <v>29686</v>
+        <v>19970</v>
       </c>
     </row>
     <row r="16">
@@ -3188,12 +3202,12 @@
       </c>
       <c r="B16" s="55" t="inlineStr">
         <is>
-          <t>26/11/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="C16" s="74" t="inlineStr">
         <is>
-          <t>27/12/2025</t>
+          <t>18/12/2025</t>
         </is>
       </c>
       <c r="D16" s="35">
@@ -3207,13 +3221,13 @@
       </c>
       <c r="H16" s="163" t="n"/>
       <c r="I16" s="28" t="n">
-        <v>808</v>
+        <v>132</v>
       </c>
       <c r="J16" s="28" t="n">
-        <v>748</v>
+        <v>132</v>
       </c>
       <c r="K16" s="28" t="n">
-        <v>848</v>
+        <v>513</v>
       </c>
       <c r="L16" s="73">
         <f>(K16+(E16-I16))</f>
@@ -3224,25 +3238,25 @@
         <v/>
       </c>
       <c r="N16" s="180" t="n">
-        <v>139.87</v>
+        <v>511.7</v>
       </c>
       <c r="O16" s="35">
         <f>I16-J16</f>
         <v/>
       </c>
       <c r="P16" s="28" t="n">
-        <v>342</v>
+        <v>0</v>
       </c>
       <c r="R16" s="140" t="inlineStr">
         <is>
-          <t>13168154-1</t>
+          <t>12378019-5</t>
         </is>
       </c>
       <c r="S16" s="140" t="n">
-        <v>29686</v>
+        <v>19970</v>
       </c>
       <c r="T16" s="140" t="n">
-        <v>30534</v>
+        <v>20483</v>
       </c>
     </row>
     <row r="17">
@@ -4115,36 +4129,42 @@
       </c>
       <c r="B16" s="55" t="inlineStr">
         <is>
-          <t>21/11/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="C16" s="74" t="inlineStr">
         <is>
-          <t>22/12/2025</t>
+          <t>19/12/2025</t>
         </is>
       </c>
       <c r="E16" s="163" t="n"/>
-      <c r="F16" s="27" t="n"/>
+      <c r="F16" s="27" t="n">
+        <v>481</v>
+      </c>
       <c r="G16" s="44">
         <f>IFERROR(F16/$E$5,"")</f>
         <v/>
       </c>
-      <c r="H16" s="27" t="n"/>
+      <c r="H16" s="27" t="n">
+        <v>0</v>
+      </c>
       <c r="I16" s="37" t="n">
         <v>0</v>
       </c>
       <c r="J16" s="180" t="n">
-        <v>268</v>
-      </c>
-      <c r="K16" s="47" t="n">
-        <v>868</v>
+        <v>627.24</v>
+      </c>
+      <c r="K16" s="47">
+        <f>H16-F16</f>
+        <v/>
       </c>
       <c r="M16" s="37">
         <f>'RESUMO '!$K$8</f>
         <v/>
       </c>
-      <c r="N16" s="24" t="n">
-        <v>763.62</v>
+      <c r="N16" s="24">
+        <f>M16*'UC GERADORA'!O16</f>
+        <v/>
       </c>
       <c r="O16" s="25">
         <f>H16</f>
@@ -4157,18 +4177,17 @@
       <c r="Q16" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>2968374-2</t>
-        </is>
-      </c>
-      <c r="S16" s="140" t="n">
-        <v>93517</v>
+      <c r="S16" s="140" t="inlineStr">
+        <is>
+          <t>12340952-7</t>
+        </is>
       </c>
       <c r="T16" s="140" t="n">
-        <v>94385</v>
-      </c>
-      <c r="U16" s="140" t="n"/>
+        <v>11694</v>
+      </c>
+      <c r="U16" s="140" t="n">
+        <v>12175</v>
+      </c>
     </row>
     <row r="17">
       <c r="E17" s="39">
@@ -4292,1131 +4311,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:T94"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="11.5546875" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
-    <col width="13.5546875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="11.88671875" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="12.5546875" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="16.33203125" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="2.6640625" customWidth="1" min="7" max="7"/>
-    <col width="14.44140625" customWidth="1" min="8" max="8"/>
-    <col width="11.33203125" customWidth="1" min="9" max="9"/>
-    <col width="14.33203125" customWidth="1" min="10" max="10"/>
-    <col width="11.6640625" customWidth="1" min="11" max="11"/>
-    <col width="13.33203125" bestFit="1" customWidth="1" min="12" max="12"/>
-    <col width="11.6640625" customWidth="1" min="13" max="13"/>
-    <col width="14.5546875" bestFit="1" customWidth="1" min="14" max="14"/>
-    <col width="16" bestFit="1" customWidth="1" min="15" max="15"/>
-    <col width="11.5546875" customWidth="1" min="16" max="16"/>
-    <col width="5" customWidth="1" min="17" max="17"/>
-    <col width="15.109375" bestFit="1" customWidth="1" min="18" max="18"/>
-    <col width="13.88671875" customWidth="1" min="19" max="19"/>
-    <col width="15" customWidth="1" min="20" max="20"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="125" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="129" t="inlineStr">
-        <is>
-          <t>UNIDADE GERADORA -</t>
-        </is>
-      </c>
-      <c r="B2" s="173" t="n"/>
-      <c r="C2" s="173" t="n"/>
-      <c r="D2" s="173" t="n"/>
-      <c r="E2" s="173" t="n"/>
-      <c r="F2" s="173" t="n"/>
-      <c r="G2" s="173" t="n"/>
-      <c r="H2" s="173" t="n"/>
-      <c r="I2" s="173" t="n"/>
-      <c r="J2" s="173" t="n"/>
-      <c r="K2" s="174">
-        <f>'RESUMO '!F7</f>
-        <v/>
-      </c>
-      <c r="L2" s="173" t="n"/>
-      <c r="M2" s="173" t="n"/>
-      <c r="N2" s="173" t="n"/>
-      <c r="O2" s="173" t="n"/>
-      <c r="P2" s="158" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="119" t="inlineStr">
-        <is>
-          <t>Mês de Ref.</t>
-        </is>
-      </c>
-      <c r="B3" s="175" t="inlineStr">
-        <is>
-          <t>Período de leitura</t>
-        </is>
-      </c>
-      <c r="C3" s="176" t="n"/>
-      <c r="D3" s="116" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Geração </t>
-        </is>
-      </c>
-      <c r="E3" s="155" t="n"/>
-      <c r="F3" s="177" t="n"/>
-      <c r="G3" s="121" t="n"/>
-      <c r="H3" s="116" t="inlineStr">
-        <is>
-          <t>Créditos</t>
-        </is>
-      </c>
-      <c r="I3" s="155" t="n"/>
-      <c r="J3" s="155" t="n"/>
-      <c r="K3" s="155" t="n"/>
-      <c r="L3" s="155" t="n"/>
-      <c r="M3" s="155" t="n"/>
-      <c r="N3" s="155" t="n"/>
-      <c r="O3" s="155" t="n"/>
-      <c r="P3" s="177" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="178" t="n"/>
-      <c r="B4" s="141" t="inlineStr">
-        <is>
-          <t>Leitura Anterior</t>
-        </is>
-      </c>
-      <c r="C4" s="142" t="inlineStr">
-        <is>
-          <t>Leitura Atual</t>
-        </is>
-      </c>
-      <c r="D4" s="33" t="inlineStr">
-        <is>
-          <t>Estimativa</t>
-        </is>
-      </c>
-      <c r="E4" s="33" t="inlineStr">
-        <is>
-          <t>Real (Solar View)</t>
-        </is>
-      </c>
-      <c r="F4" s="33" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="H4" s="38" t="inlineStr">
-        <is>
-          <t>Consumo médio</t>
-        </is>
-      </c>
-      <c r="I4" s="48" t="inlineStr">
-        <is>
-          <t>Energia GERAÇÃO</t>
-        </is>
-      </c>
-      <c r="J4" s="48" t="inlineStr">
-        <is>
-          <t>ENREGIA COMPENSADA</t>
-        </is>
-      </c>
-      <c r="K4" s="48" t="inlineStr">
-        <is>
-          <t>ENERGIA ATIVA</t>
-        </is>
-      </c>
-      <c r="L4" s="38" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Consumo Real </t>
-        </is>
-      </c>
-      <c r="M4" s="38" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="N4" s="12" t="inlineStr">
-        <is>
-          <t>VALOR FATURA</t>
-        </is>
-      </c>
-      <c r="O4" s="33" t="inlineStr">
-        <is>
-          <t>Mensal (Crédito)</t>
-        </is>
-      </c>
-      <c r="P4" s="48" t="inlineStr">
-        <is>
-          <t>Conferência (Crédito da Fatura) (Olho em saldo na fatura GERADORA, o valor tem que bater com o "Mensal (coluna do lado)" se não tem alguma coisa errada na Equatorial ou na planilha, caso seja na Equatorial, tenho que ligar lá)</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="R4" s="145" t="inlineStr">
-        <is>
-          <t>LEITURA DO MEDIDOR</t>
-        </is>
-      </c>
-      <c r="S4" s="173" t="n"/>
-      <c r="T4" s="158" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="122" t="inlineStr">
-        <is>
-          <t>Jan</t>
-        </is>
-      </c>
-      <c r="B5" s="74" t="inlineStr">
-        <is>
-          <t>04/12/2024</t>
-        </is>
-      </c>
-      <c r="C5" s="74" t="inlineStr">
-        <is>
-          <t>03/01/2025</t>
-        </is>
-      </c>
-      <c r="D5" s="35">
-        <f>'RESUMO '!B14</f>
-        <v/>
-      </c>
-      <c r="E5" s="28" t="n"/>
-      <c r="F5" s="34">
-        <f>IFERROR(E5/D5-1,"")</f>
-        <v/>
-      </c>
-      <c r="H5" s="179">
-        <f>'RESUMO '!I7</f>
-        <v/>
-      </c>
-      <c r="I5" s="28" t="n">
-        <v>1353</v>
-      </c>
-      <c r="J5" s="28" t="n">
-        <v>767</v>
-      </c>
-      <c r="K5" s="28" t="n">
-        <v>867</v>
-      </c>
-      <c r="L5" s="73">
-        <f>(K5+(E5-I5))</f>
-        <v/>
-      </c>
-      <c r="M5" s="44">
-        <f>IFERROR(L5/$H$5,"")</f>
-        <v/>
-      </c>
-      <c r="N5" s="180" t="n">
-        <v>243.85</v>
-      </c>
-      <c r="O5" s="35">
-        <f>I5-J5</f>
-        <v/>
-      </c>
-      <c r="P5" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" s="146" t="inlineStr">
-        <is>
-          <t>12774111-9</t>
-        </is>
-      </c>
-      <c r="S5" s="146" t="n">
-        <v>35335</v>
-      </c>
-      <c r="T5" s="146" t="n">
-        <v>36202</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="122" t="inlineStr">
-        <is>
-          <t>Fev</t>
-        </is>
-      </c>
-      <c r="B6" s="55" t="inlineStr">
-        <is>
-          <t>03/01/2025</t>
-        </is>
-      </c>
-      <c r="C6" s="74" t="inlineStr">
-        <is>
-          <t>04/02/2025</t>
-        </is>
-      </c>
-      <c r="D6" s="35">
-        <f>'RESUMO '!B15</f>
-        <v/>
-      </c>
-      <c r="E6" s="28" t="n"/>
-      <c r="F6" s="34">
-        <f>IFERROR(E6/D6-1,"")</f>
-        <v/>
-      </c>
-      <c r="H6" s="181" t="n"/>
-      <c r="I6" s="28" t="n">
-        <v>1346</v>
-      </c>
-      <c r="J6" s="28" t="n">
-        <v>815</v>
-      </c>
-      <c r="K6" s="28" t="n">
-        <v>915</v>
-      </c>
-      <c r="L6" s="73">
-        <f>(K6+(E6-I6))</f>
-        <v/>
-      </c>
-      <c r="M6" s="44">
-        <f>IFERROR(L6/$H$5,"")</f>
-        <v/>
-      </c>
-      <c r="N6" s="180" t="n">
-        <v>113.9</v>
-      </c>
-      <c r="O6" s="35">
-        <f>I6-J6</f>
-        <v/>
-      </c>
-      <c r="P6" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="140" t="inlineStr">
-        <is>
-          <t>12774111-9</t>
-        </is>
-      </c>
-      <c r="S6" s="140" t="n">
-        <v>36202</v>
-      </c>
-      <c r="T6" s="140" t="n">
-        <v>37117</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="122" t="inlineStr">
-        <is>
-          <t>Mar</t>
-        </is>
-      </c>
-      <c r="B7" s="55" t="inlineStr">
-        <is>
-          <t>04/02/2025</t>
-        </is>
-      </c>
-      <c r="C7" s="74" t="inlineStr">
-        <is>
-          <t>05/03/2025</t>
-        </is>
-      </c>
-      <c r="D7" s="35">
-        <f>'RESUMO '!B16</f>
-        <v/>
-      </c>
-      <c r="E7" s="28" t="n"/>
-      <c r="F7" s="34">
-        <f>IFERROR(E7/D7-1,"")</f>
-        <v/>
-      </c>
-      <c r="H7" s="181" t="n"/>
-      <c r="I7" s="28" t="n">
-        <v>1281</v>
-      </c>
-      <c r="J7" s="28" t="n">
-        <v>861</v>
-      </c>
-      <c r="K7" s="28" t="n">
-        <v>961</v>
-      </c>
-      <c r="L7" s="73">
-        <f>(K7+(E7-I7))</f>
-        <v/>
-      </c>
-      <c r="M7" s="44">
-        <f>IFERROR(L7/$H$5,"")</f>
-        <v/>
-      </c>
-      <c r="N7" s="180" t="n">
-        <v>113.74</v>
-      </c>
-      <c r="O7" s="35">
-        <f>I7-J7</f>
-        <v/>
-      </c>
-      <c r="P7" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" s="140" t="inlineStr">
-        <is>
-          <t>12774111-9</t>
-        </is>
-      </c>
-      <c r="S7" s="140" t="n">
-        <v>37117</v>
-      </c>
-      <c r="T7" s="140" t="n">
-        <v>38078</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="122" t="inlineStr">
-        <is>
-          <t>Abr</t>
-        </is>
-      </c>
-      <c r="B8" s="55" t="inlineStr">
-        <is>
-          <t>05/03/2025</t>
-        </is>
-      </c>
-      <c r="C8" s="74" t="inlineStr">
-        <is>
-          <t>02/04/2025</t>
-        </is>
-      </c>
-      <c r="D8" s="35">
-        <f>'RESUMO '!B17</f>
-        <v/>
-      </c>
-      <c r="E8" s="28" t="n"/>
-      <c r="F8" s="34">
-        <f>IFERROR(E8/D8-1,"")</f>
-        <v/>
-      </c>
-      <c r="H8" s="181" t="n"/>
-      <c r="I8" s="28" t="n">
-        <v>1004</v>
-      </c>
-      <c r="J8" s="28" t="n">
-        <v>941</v>
-      </c>
-      <c r="K8" s="28" t="n">
-        <v>1041</v>
-      </c>
-      <c r="L8" s="73">
-        <f>(K8+(E8-I8))</f>
-        <v/>
-      </c>
-      <c r="M8" s="44">
-        <f>IFERROR(L8/$H$5,"")</f>
-        <v/>
-      </c>
-      <c r="N8" s="180" t="n">
-        <v>118.77</v>
-      </c>
-      <c r="O8" s="35">
-        <f>I8-J8</f>
-        <v/>
-      </c>
-      <c r="P8" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" s="140" t="inlineStr">
-        <is>
-          <t>12774111-9</t>
-        </is>
-      </c>
-      <c r="S8" s="140" t="n">
-        <v>38078</v>
-      </c>
-      <c r="T8" s="140" t="n">
-        <v>39119</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="122" t="inlineStr">
-        <is>
-          <t>Mai</t>
-        </is>
-      </c>
-      <c r="B9" s="55" t="inlineStr">
-        <is>
-          <t>02/04/2025</t>
-        </is>
-      </c>
-      <c r="C9" s="74" t="inlineStr">
-        <is>
-          <t>02/05/2025</t>
-        </is>
-      </c>
-      <c r="D9" s="35">
-        <f>'RESUMO '!B18</f>
-        <v/>
-      </c>
-      <c r="E9" s="28" t="n"/>
-      <c r="F9" s="34">
-        <f>IFERROR(E9/D9-1,"")</f>
-        <v/>
-      </c>
-      <c r="H9" s="181" t="n"/>
-      <c r="I9" s="28" t="n">
-        <v>964</v>
-      </c>
-      <c r="J9" s="28" t="n">
-        <v>869</v>
-      </c>
-      <c r="K9" s="28" t="n">
-        <v>969</v>
-      </c>
-      <c r="L9" s="73">
-        <f>(K9+(E9-I9))</f>
-        <v/>
-      </c>
-      <c r="M9" s="44">
-        <f>IFERROR(L9/$H$5,"")</f>
-        <v/>
-      </c>
-      <c r="N9" s="180" t="n">
-        <v>110.24</v>
-      </c>
-      <c r="O9" s="35">
-        <f>I9-J9</f>
-        <v/>
-      </c>
-      <c r="P9" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" s="140" t="inlineStr">
-        <is>
-          <t>12774111-9</t>
-        </is>
-      </c>
-      <c r="S9" s="140" t="n">
-        <v>39119</v>
-      </c>
-      <c r="T9" s="140" t="n">
-        <v>40088</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="122" t="inlineStr">
-        <is>
-          <t>Jun</t>
-        </is>
-      </c>
-      <c r="B10" s="55" t="inlineStr">
-        <is>
-          <t>02/05/2025</t>
-        </is>
-      </c>
-      <c r="C10" s="74" t="inlineStr">
-        <is>
-          <t>03/06/2025</t>
-        </is>
-      </c>
-      <c r="D10" s="35">
-        <f>'RESUMO '!B19</f>
-        <v/>
-      </c>
-      <c r="E10" s="28" t="n"/>
-      <c r="F10" s="34">
-        <f>IFERROR(E10/D10-1,"")</f>
-        <v/>
-      </c>
-      <c r="H10" s="181" t="n"/>
-      <c r="I10" s="28" t="n">
-        <v>1025</v>
-      </c>
-      <c r="J10" s="28" t="n">
-        <v>815</v>
-      </c>
-      <c r="K10" s="28" t="n">
-        <v>915</v>
-      </c>
-      <c r="L10" s="73">
-        <f>(K10+(E10-I10))</f>
-        <v/>
-      </c>
-      <c r="M10" s="44">
-        <f>IFERROR(L10/$H$5,"")</f>
-        <v/>
-      </c>
-      <c r="N10" s="180" t="n">
-        <v>115.08</v>
-      </c>
-      <c r="O10" s="35">
-        <f>I10-J10</f>
-        <v/>
-      </c>
-      <c r="P10" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" s="140" t="inlineStr">
-        <is>
-          <t>12774111-9</t>
-        </is>
-      </c>
-      <c r="S10" s="140" t="n">
-        <v>40088</v>
-      </c>
-      <c r="T10" s="140" t="n">
-        <v>41003</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="122" t="inlineStr">
-        <is>
-          <t>Jul</t>
-        </is>
-      </c>
-      <c r="B11" s="55" t="inlineStr">
-        <is>
-          <t>03/06/2025</t>
-        </is>
-      </c>
-      <c r="C11" s="74" t="inlineStr">
-        <is>
-          <t>05/07/2025</t>
-        </is>
-      </c>
-      <c r="D11" s="35">
-        <f>'RESUMO '!B20</f>
-        <v/>
-      </c>
-      <c r="E11" s="28" t="n"/>
-      <c r="F11" s="34">
-        <f>IFERROR(E11/D11-1,"")</f>
-        <v/>
-      </c>
-      <c r="H11" s="181" t="n"/>
-      <c r="I11" s="28" t="n">
-        <v>871</v>
-      </c>
-      <c r="J11" s="28" t="n">
-        <v>814</v>
-      </c>
-      <c r="K11" s="28" t="n">
-        <v>914</v>
-      </c>
-      <c r="L11" s="73">
-        <f>(K11+(E11-I11))</f>
-        <v/>
-      </c>
-      <c r="M11" s="44">
-        <f>IFERROR(L11/$H$5,"")</f>
-        <v/>
-      </c>
-      <c r="N11" s="180" t="n">
-        <v>115.11</v>
-      </c>
-      <c r="O11" s="35">
-        <f>I11-J11</f>
-        <v/>
-      </c>
-      <c r="P11" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" s="140" t="inlineStr">
-        <is>
-          <t>12774111-9</t>
-        </is>
-      </c>
-      <c r="S11" s="140" t="n">
-        <v>41003</v>
-      </c>
-      <c r="T11" s="140" t="n">
-        <v>41917</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="122" t="inlineStr">
-        <is>
-          <t>Ago</t>
-        </is>
-      </c>
-      <c r="B12" s="55" t="inlineStr">
-        <is>
-          <t>05/07/2025</t>
-        </is>
-      </c>
-      <c r="C12" s="74" t="inlineStr">
-        <is>
-          <t>02/08/2025</t>
-        </is>
-      </c>
-      <c r="D12" s="35">
-        <f>'RESUMO '!B21</f>
-        <v/>
-      </c>
-      <c r="E12" s="28" t="n"/>
-      <c r="F12" s="34">
-        <f>IFERROR(E12/D12-1,"")</f>
-        <v/>
-      </c>
-      <c r="H12" s="181" t="n"/>
-      <c r="I12" s="28" t="n">
-        <v>718</v>
-      </c>
-      <c r="J12" s="28" t="n">
-        <v>718</v>
-      </c>
-      <c r="K12" s="28" t="n">
-        <v>873</v>
-      </c>
-      <c r="L12" s="73">
-        <f>(K12+(E12-I12))</f>
-        <v/>
-      </c>
-      <c r="M12" s="44">
-        <f>IFERROR(L12/$H$5,"")</f>
-        <v/>
-      </c>
-      <c r="N12" s="180" t="n">
-        <v>174.2</v>
-      </c>
-      <c r="O12" s="35">
-        <f>I12-J12</f>
-        <v/>
-      </c>
-      <c r="P12" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" s="140" t="inlineStr">
-        <is>
-          <t>12774111-9</t>
-        </is>
-      </c>
-      <c r="S12" s="140" t="n">
-        <v>41917</v>
-      </c>
-      <c r="T12" s="140" t="n">
-        <v>42790</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="122" t="inlineStr">
-        <is>
-          <t>Set</t>
-        </is>
-      </c>
-      <c r="B13" s="55" t="inlineStr">
-        <is>
-          <t>02/08/2025</t>
-        </is>
-      </c>
-      <c r="C13" s="74" t="inlineStr">
-        <is>
-          <t>02/09/2025</t>
-        </is>
-      </c>
-      <c r="D13" s="35">
-        <f>'RESUMO '!B22</f>
-        <v/>
-      </c>
-      <c r="E13" s="28" t="n"/>
-      <c r="F13" s="34">
-        <f>IFERROR(E13/D13-1,"")</f>
-        <v/>
-      </c>
-      <c r="H13" s="181" t="n"/>
-      <c r="I13" s="28" t="n">
-        <v>748</v>
-      </c>
-      <c r="J13" s="28" t="n">
-        <v>748</v>
-      </c>
-      <c r="K13" s="28" t="n">
-        <v>990</v>
-      </c>
-      <c r="L13" s="73">
-        <f>(K13+(E13-I13))</f>
-        <v/>
-      </c>
-      <c r="M13" s="44">
-        <f>IFERROR(L13/$H$5,"")</f>
-        <v/>
-      </c>
-      <c r="N13" s="180" t="n">
-        <v>271.68</v>
-      </c>
-      <c r="O13" s="35">
-        <f>I13-J13</f>
-        <v/>
-      </c>
-      <c r="P13" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" s="140" t="inlineStr">
-        <is>
-          <t>12774111-9</t>
-        </is>
-      </c>
-      <c r="S13" s="140" t="n">
-        <v>42790</v>
-      </c>
-      <c r="T13" s="140" t="n">
-        <v>43780</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="122" t="inlineStr">
-        <is>
-          <t>Out</t>
-        </is>
-      </c>
-      <c r="B14" s="55" t="inlineStr">
-        <is>
-          <t>02/09/2025</t>
-        </is>
-      </c>
-      <c r="C14" s="74" t="inlineStr">
-        <is>
-          <t>02/10/2025</t>
-        </is>
-      </c>
-      <c r="D14" s="35">
-        <f>'RESUMO '!B23</f>
-        <v/>
-      </c>
-      <c r="E14" s="71" t="n"/>
-      <c r="F14" s="34">
-        <f>IFERROR(E14/D14-1,"")</f>
-        <v/>
-      </c>
-      <c r="H14" s="181" t="n"/>
-      <c r="I14" s="28" t="n">
-        <v>899</v>
-      </c>
-      <c r="J14" s="28" t="n">
-        <v>899</v>
-      </c>
-      <c r="K14" s="28" t="n">
-        <v>1083</v>
-      </c>
-      <c r="L14" s="73">
-        <f>(K14+(E14-I14))</f>
-        <v/>
-      </c>
-      <c r="M14" s="44">
-        <f>IFERROR(L14/$H$5,"")</f>
-        <v/>
-      </c>
-      <c r="N14" s="180" t="n">
-        <v>233.85</v>
-      </c>
-      <c r="O14" s="35">
-        <f>I14-J14</f>
-        <v/>
-      </c>
-      <c r="P14" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" s="140" t="inlineStr">
-        <is>
-          <t>12774111-9</t>
-        </is>
-      </c>
-      <c r="S14" s="140" t="n">
-        <v>43780</v>
-      </c>
-      <c r="T14" s="140" t="n">
-        <v>44863</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="122" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="B15" s="55" t="inlineStr">
-        <is>
-          <t>02/10/2025</t>
-        </is>
-      </c>
-      <c r="C15" s="74" t="inlineStr">
-        <is>
-          <t>03/11/2025</t>
-        </is>
-      </c>
-      <c r="D15" s="35">
-        <f>'RESUMO '!B24</f>
-        <v/>
-      </c>
-      <c r="E15" s="28" t="n"/>
-      <c r="F15" s="34">
-        <f>IFERROR(E15/D15-1,"")</f>
-        <v/>
-      </c>
-      <c r="H15" s="181" t="n"/>
-      <c r="I15" s="28" t="n">
-        <v>1071</v>
-      </c>
-      <c r="J15" s="28" t="n">
-        <v>71</v>
-      </c>
-      <c r="K15" s="28" t="n">
-        <v>1259</v>
-      </c>
-      <c r="L15" s="73">
-        <f>(K15+(E15-I15))</f>
-        <v/>
-      </c>
-      <c r="M15" s="44">
-        <f>IFERROR(L15/$H$5,"")</f>
-        <v/>
-      </c>
-      <c r="N15" s="180" t="n">
-        <v>234.97</v>
-      </c>
-      <c r="O15" s="35">
-        <f>I15-J15</f>
-        <v/>
-      </c>
-      <c r="P15" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R15" s="140" t="inlineStr">
-        <is>
-          <t>12774111-9</t>
-        </is>
-      </c>
-      <c r="S15" s="140" t="n">
-        <v>44863</v>
-      </c>
-      <c r="T15" s="140" t="n">
-        <v>46122</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="122" t="inlineStr">
-        <is>
-          <t>Dez</t>
-        </is>
-      </c>
-      <c r="B16" s="55" t="inlineStr">
-        <is>
-          <t>03/11/2025</t>
-        </is>
-      </c>
-      <c r="C16" s="74" t="inlineStr">
-        <is>
-          <t>05/12/2025</t>
-        </is>
-      </c>
-      <c r="D16" s="35">
-        <f>'RESUMO '!B25</f>
-        <v/>
-      </c>
-      <c r="E16" s="28" t="n"/>
-      <c r="F16" s="34">
-        <f>IFERROR(E16/D16-1,"")</f>
-        <v/>
-      </c>
-      <c r="H16" s="163" t="n"/>
-      <c r="I16" s="28" t="n">
-        <v>302</v>
-      </c>
-      <c r="J16" s="28" t="n">
-        <v>302</v>
-      </c>
-      <c r="K16" s="28" t="n">
-        <v>2051</v>
-      </c>
-      <c r="L16" s="73">
-        <f>(K16+(E16-I16))</f>
-        <v/>
-      </c>
-      <c r="M16" s="44">
-        <f>IFERROR(L16/$H$5,"")</f>
-        <v/>
-      </c>
-      <c r="N16" s="180" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" s="35">
-        <f>I16-J16</f>
-        <v/>
-      </c>
-      <c r="P16" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" s="140" t="inlineStr">
-        <is>
-          <t>12774111-9</t>
-        </is>
-      </c>
-      <c r="S16" s="140" t="n">
-        <v>46122</v>
-      </c>
-      <c r="T16" s="140" t="n">
-        <v>48173</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="32" t="inlineStr">
-        <is>
-          <t>∑</t>
-        </is>
-      </c>
-      <c r="B17" s="122" t="inlineStr">
-        <is>
-          <t xml:space="preserve">TOTAL </t>
-        </is>
-      </c>
-      <c r="C17" s="158" t="n"/>
-      <c r="D17" s="35">
-        <f>SUM(D5:D16)</f>
-        <v/>
-      </c>
-      <c r="E17" s="35">
-        <f>SUM(E5:E16)</f>
-        <v/>
-      </c>
-      <c r="F17" s="34">
-        <f>IFERROR(E17/D17-1,"")</f>
-        <v/>
-      </c>
-      <c r="H17" s="45">
-        <f>H5*12</f>
-        <v/>
-      </c>
-      <c r="I17" s="35">
-        <f>IFERROR(AVERAGE(I5:I16),"")</f>
-        <v/>
-      </c>
-      <c r="J17" s="35">
-        <f>IFERROR(AVERAGE(J5:J16),"")</f>
-        <v/>
-      </c>
-      <c r="K17" s="35">
-        <f>IFERROR(AVERAGE(K5:K16),"")</f>
-        <v/>
-      </c>
-      <c r="L17" s="35">
-        <f>SUM(L5:L16)</f>
-        <v/>
-      </c>
-      <c r="M17" s="44">
-        <f>IFERROR(L17/$H$5,"")</f>
-        <v/>
-      </c>
-      <c r="N17" s="31">
-        <f>SUM(N5:N16)</f>
-        <v/>
-      </c>
-      <c r="O17" s="35">
-        <f>SUM(O5:O16)</f>
-        <v/>
-      </c>
-      <c r="P17" s="35">
-        <f>SUM(P5:P16)</f>
-        <v/>
-      </c>
-      <c r="R17" s="140" t="n"/>
-      <c r="S17" s="140" t="n"/>
-      <c r="T17" s="140" t="n"/>
-    </row>
-    <row r="18">
-      <c r="D18" s="122" t="inlineStr">
-        <is>
-          <t>Média =</t>
-        </is>
-      </c>
-      <c r="E18" s="72">
-        <f>AVERAGE(E5:E16)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="115" t="inlineStr">
-        <is>
-          <t>LEGENDA</t>
-        </is>
-      </c>
-      <c r="B19" s="173" t="n"/>
-      <c r="C19" s="158" t="n"/>
-      <c r="H19" s="124" t="inlineStr">
-        <is>
-          <t>Obs:. Para Calcular a média de consumo real utilize a forumula -&gt;</t>
-        </is>
-      </c>
-      <c r="L19">
-        <f>AVERAGEIF(L5:L16, "&lt;&gt;0")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>AMARELO</t>
-        </is>
-      </c>
-      <c r="B20" s="21" t="inlineStr">
-        <is>
-          <t>PREENCHER</t>
-        </is>
-      </c>
-      <c r="C20" s="21" t="n"/>
-      <c r="I20" s="123" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="17" t="inlineStr">
-        <is>
-          <t>CINZA</t>
-        </is>
-      </c>
-      <c r="B21" s="22" t="inlineStr">
-        <is>
-          <t>AUTOMÁTICO</t>
-        </is>
-      </c>
-      <c r="C21" s="22" t="n"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="36" t="inlineStr">
-        <is>
-          <t>LARANJA</t>
-        </is>
-      </c>
-      <c r="B22" s="182" t="inlineStr">
-        <is>
-          <t>COBRAR</t>
-        </is>
-      </c>
-      <c r="C22" s="158" t="n"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="54" t="n"/>
-    </row>
-    <row r="94">
-      <c r="O94" s="1" t="n"/>
-    </row>
-  </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="K2:P2"/>
-    <mergeCell ref="H5:H16"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="G3:G17"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="H3:P3"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="H19:K19"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
-</worksheet>
 </file>
</xml_diff>